<commit_message>
++ update file template import partner
</commit_message>
<xml_diff>
--- a/WebAPI/eFMS.API.SystemWeb/eFMS.API.Catalogue/eFMS.API.Catalogue/Resources/Files/PartnerImportTemplate.xlsx
+++ b/WebAPI/eFMS.API.SystemWeb/eFMS.API.Catalogue/eFMS.API.Catalogue/Resources/Files/PartnerImportTemplate.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\samuel.an\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\samuel.an\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -84,7 +84,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="57">
   <si>
     <t>Zipcode</t>
   </si>
@@ -161,9 +161,6 @@
     <t>Partner Mode</t>
   </si>
   <si>
-    <t>Internal</t>
-  </si>
-  <si>
     <t>Internal Code</t>
   </si>
   <si>
@@ -233,9 +230,6 @@
     <t>Apply For Dim</t>
   </si>
   <si>
-    <t>Shipping Address EN</t>
-  </si>
-  <si>
     <t>Shipping Address Local</t>
   </si>
   <si>
@@ -254,7 +248,13 @@
     <t>Name Local</t>
   </si>
   <si>
-    <t>3123123123 i9</t>
+    <t>Credit Payment</t>
+  </si>
+  <si>
+    <t>Direct</t>
+  </si>
+  <si>
+    <t>External</t>
   </si>
 </sst>
 </file>
@@ -644,10 +644,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AI2"/>
+  <dimension ref="A1:AJ2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -659,7 +659,7 @@
     <col min="5" max="8" width="20" customWidth="1"/>
     <col min="9" max="9" width="18" customWidth="1"/>
     <col min="10" max="11" width="17.42578125" customWidth="1"/>
-    <col min="12" max="12" width="37.5703125" customWidth="1"/>
+    <col min="12" max="12" width="21.5703125" customWidth="1"/>
     <col min="13" max="13" width="28.5703125" customWidth="1"/>
     <col min="14" max="14" width="15.85546875" customWidth="1"/>
     <col min="15" max="15" width="16.5703125" customWidth="1"/>
@@ -677,21 +677,21 @@
     <col min="34" max="34" width="12.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" s="5" customFormat="1" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:36" s="5" customFormat="1" ht="28.5" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="C1" s="3" t="s">
         <v>42</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>43</v>
       </c>
       <c r="D1" s="4" t="s">
         <v>21</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F1" s="3" t="s">
         <v>23</v>
@@ -700,109 +700,112 @@
         <v>24</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I1" s="3" t="s">
         <v>19</v>
       </c>
       <c r="J1" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="M1" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="N1" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="O1" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="P1" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q1" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="R1" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="S1" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="T1" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="U1" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="V1" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="W1" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="X1" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="Y1" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="Z1" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="AA1" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="AB1" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="AC1" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="AD1" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="K1" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="L1" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="M1" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="N1" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="O1" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="P1" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="Q1" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="R1" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="S1" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="T1" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="U1" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="V1" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="W1" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="X1" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="Y1" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="Z1" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="AA1" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="AB1" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="AC1" s="7" t="s">
+      <c r="AE1" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="AF1" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="AG1" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="AH1" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="AD1" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="AE1" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="AF1" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="AG1" s="8" t="s">
+      <c r="AI1" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="AH1" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="AI1" s="7" t="s">
+      <c r="AJ1" s="7" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>53</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>55</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="E2" s="1" t="s">
-        <v>56</v>
+      <c r="E2" s="1">
+        <v>659885474</v>
       </c>
       <c r="F2" s="1"/>
       <c r="G2" s="1" t="s">
-        <v>25</v>
+        <v>56</v>
       </c>
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
@@ -813,29 +816,31 @@
         <v>222</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="N2" s="1" t="s">
         <v>18</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="P2" s="1"/>
+        <v>18</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>37</v>
+      </c>
       <c r="Q2" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="R2" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="S2" s="1" t="s">
         <v>18</v>
       </c>
       <c r="T2" s="1" t="s">
-        <v>38</v>
+        <v>18</v>
       </c>
       <c r="U2" s="1"/>
       <c r="V2" s="1"/>
@@ -854,7 +859,7 @@
       <c r="AI2" s="2"/>
     </row>
   </sheetData>
-  <dataValidations count="4">
+  <dataValidations count="5">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2">
       <formula1>"Domestic,Oversea"</formula1>
     </dataValidation>
@@ -866,6 +871,9 @@
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AG2">
       <formula1>"Standard,Round 0.5, Round 1.0"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L2">
+      <formula1>"Credit,Direct"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -879,7 +887,7 @@
   <dimension ref="B2:D11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>